<commit_message>
updating the formatted pivots
</commit_message>
<xml_diff>
--- a/Tables/Formatted/Journal Pivot.xlsx
+++ b/Tables/Formatted/Journal Pivot.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gorbetw\Desktop\GPT Detection\Pivots\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gorbetw\Documents\Repos\AI-Detection\Tables\Formatted\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8505"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12885"/>
   </bookViews>
   <sheets>
     <sheet name="journal-pivot" sheetId="1" r:id="rId1"/>
@@ -1013,7 +1013,7 @@
   <dimension ref="B2:H7"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+      <selection activeCell="C4" sqref="C4:H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1052,22 +1052,22 @@
         <v>6</v>
       </c>
       <c r="C3" s="6">
-        <v>52</v>
+        <v>83</v>
       </c>
       <c r="D3" s="6">
+        <v>25</v>
+      </c>
+      <c r="E3" s="6">
+        <v>17</v>
+      </c>
+      <c r="F3" s="6">
+        <v>20</v>
+      </c>
+      <c r="G3" s="6">
         <v>16</v>
       </c>
-      <c r="E3" s="6">
-        <v>9</v>
-      </c>
-      <c r="F3" s="6">
-        <v>7</v>
-      </c>
-      <c r="G3" s="6">
-        <v>8</v>
-      </c>
       <c r="H3" s="6">
-        <v>1308</v>
+        <v>2512</v>
       </c>
     </row>
     <row r="4" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1075,22 +1075,22 @@
         <v>7</v>
       </c>
       <c r="C4" s="6">
+        <v>105</v>
+      </c>
+      <c r="D4" s="6">
         <v>28</v>
       </c>
-      <c r="D4" s="6">
-        <v>6</v>
-      </c>
       <c r="E4" s="6">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="F4" s="6">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="G4" s="6">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="H4" s="6">
-        <v>1349</v>
+        <v>5371</v>
       </c>
     </row>
     <row r="5" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1098,22 +1098,22 @@
         <v>8</v>
       </c>
       <c r="C5" s="6">
-        <v>34</v>
+        <v>57</v>
       </c>
       <c r="D5" s="6">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="E5" s="6">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="F5" s="6">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="G5" s="6">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="H5" s="6">
-        <v>1333</v>
+        <v>2816</v>
       </c>
     </row>
     <row r="6" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1121,22 +1121,22 @@
         <v>9</v>
       </c>
       <c r="C6" s="6">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="D6" s="6">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E6" s="6">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F6" s="6">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="G6" s="6">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H6" s="6">
-        <v>1313</v>
+        <v>1015</v>
       </c>
     </row>
     <row r="7" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1144,22 +1144,22 @@
         <v>10</v>
       </c>
       <c r="C7" s="6">
-        <v>136</v>
+        <v>220</v>
       </c>
       <c r="D7" s="6">
-        <v>23</v>
+        <v>39</v>
       </c>
       <c r="E7" s="6">
+        <v>28</v>
+      </c>
+      <c r="F7" s="6">
+        <v>24</v>
+      </c>
+      <c r="G7" s="6">
         <v>18</v>
       </c>
-      <c r="F7" s="6">
-        <v>11</v>
-      </c>
-      <c r="G7" s="6">
-        <v>12</v>
-      </c>
       <c r="H7" s="6">
-        <v>1200</v>
+        <v>1820</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updates to tables, images of tables new word distribution graph updates to paper
</commit_message>
<xml_diff>
--- a/Tables/Formatted/Journal Pivot.xlsx
+++ b/Tables/Formatted/Journal Pivot.xlsx
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="journal-pivot" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -204,7 +204,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="40">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -384,8 +384,50 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA3D0EF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC693"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF9FE59F"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF0AAAA"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD8C7E7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.749992370372631"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="10">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -500,6 +542,50 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -545,7 +631,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -553,16 +639,46 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="34" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="35" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="36" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="37" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="38" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="34" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="35" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="36" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="37" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="38" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="39" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="39" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="33" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="33" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -623,7 +739,27 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal style="thin">
+          <color auto="1"/>
+        </horizontal>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -637,7 +773,27 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFD8C7E7"/>
+        </patternFill>
+      </fill>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal style="thin">
+          <color auto="1"/>
+        </horizontal>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -651,7 +807,27 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFF0AAAA"/>
+        </patternFill>
+      </fill>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal style="thin">
+          <color auto="1"/>
+        </horizontal>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -665,7 +841,27 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FF9FE59F"/>
+        </patternFill>
+      </fill>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal style="thin">
+          <color auto="1"/>
+        </horizontal>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -679,7 +875,27 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFFC693"/>
+        </patternFill>
+      </fill>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal style="thin">
+          <color auto="1"/>
+        </horizontal>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -693,27 +909,86 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFA3D0EF"/>
+        </patternFill>
+      </fill>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal style="thin">
+          <color auto="1"/>
+        </horizontal>
+      </border>
     </dxf>
     <dxf>
       <font>
         <b/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
       </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="2" tint="-0.749992370372631"/>
+        </patternFill>
+      </fill>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <border diagonalUp="0" diagonalDown="0">
-        <left/>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
         <right style="thick">
           <color auto="1"/>
         </right>
-        <top/>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
         <bottom style="thick">
           <color auto="1"/>
         </bottom>
       </border>
     </dxf>
     <dxf>
+      <font>
+        <b/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="1" tint="0.249977111117893"/>
+        </patternFill>
+      </fill>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -721,6 +996,15 @@
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFD8C7E7"/>
+      <color rgb="FFF0AAAA"/>
+      <color rgb="FF9FE59F"/>
+      <color rgb="FFFFC693"/>
+      <color rgb="FFA3D0EF"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -733,7 +1017,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="B2:H7" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8" tableBorderDxfId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="B2:H7" totalsRowShown="0" headerRowDxfId="8" dataDxfId="9" tableBorderDxfId="7">
   <tableColumns count="7">
     <tableColumn id="1" name="Journal" dataDxfId="6"/>
     <tableColumn id="2" name="Greater than 90% chance of being AI generated" dataDxfId="5"/>
@@ -743,7 +1027,7 @@
     <tableColumn id="6" name="Greater than 50% chance of being AI generated" dataDxfId="1"/>
     <tableColumn id="7" name="Less than 50% chance of being AI generated" dataDxfId="0"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -1010,7 +1294,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:H7"/>
+  <dimension ref="B2:H8"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
@@ -1025,143 +1309,144 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="G2" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="H2" s="14" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="3" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="6">
+      <c r="C3" s="15">
         <v>83</v>
       </c>
-      <c r="D3" s="6">
+      <c r="D3" s="3">
         <v>25</v>
       </c>
-      <c r="E3" s="6">
+      <c r="E3" s="4">
         <v>17</v>
       </c>
-      <c r="F3" s="6">
+      <c r="F3" s="5">
         <v>20</v>
       </c>
       <c r="G3" s="6">
         <v>16</v>
       </c>
-      <c r="H3" s="6">
+      <c r="H3" s="7">
         <v>2512</v>
       </c>
     </row>
     <row r="4" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="6">
+      <c r="C4" s="15">
         <v>105</v>
       </c>
-      <c r="D4" s="6">
+      <c r="D4" s="3">
         <v>28</v>
       </c>
-      <c r="E4" s="6">
+      <c r="E4" s="4">
         <v>17</v>
       </c>
-      <c r="F4" s="6">
+      <c r="F4" s="5">
         <v>17</v>
       </c>
       <c r="G4" s="6">
         <v>17</v>
       </c>
-      <c r="H4" s="6">
+      <c r="H4" s="7">
         <v>5371</v>
       </c>
     </row>
     <row r="5" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="6">
+      <c r="C5" s="15">
         <v>57</v>
       </c>
-      <c r="D5" s="6">
+      <c r="D5" s="3">
         <v>17</v>
       </c>
-      <c r="E5" s="6">
+      <c r="E5" s="4">
         <v>13</v>
       </c>
-      <c r="F5" s="6">
+      <c r="F5" s="5">
         <v>17</v>
       </c>
       <c r="G5" s="6">
         <v>22</v>
       </c>
-      <c r="H5" s="6">
+      <c r="H5" s="7">
         <v>2816</v>
       </c>
     </row>
     <row r="6" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="6">
+      <c r="C6" s="15">
         <v>42</v>
       </c>
-      <c r="D6" s="6">
+      <c r="D6" s="3">
         <v>9</v>
       </c>
-      <c r="E6" s="6">
+      <c r="E6" s="4">
         <v>2</v>
       </c>
-      <c r="F6" s="6">
+      <c r="F6" s="5">
         <v>6</v>
       </c>
       <c r="G6" s="6">
         <v>7</v>
       </c>
-      <c r="H6" s="6">
+      <c r="H6" s="7">
         <v>1015</v>
       </c>
     </row>
     <row r="7" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="6">
+      <c r="C7" s="16">
         <v>220</v>
       </c>
-      <c r="D7" s="6">
+      <c r="D7" s="8">
         <v>39</v>
       </c>
-      <c r="E7" s="6">
+      <c r="E7" s="9">
         <v>28</v>
       </c>
-      <c r="F7" s="6">
+      <c r="F7" s="10">
         <v>24</v>
       </c>
-      <c r="G7" s="6">
+      <c r="G7" s="11">
         <v>18</v>
       </c>
-      <c r="H7" s="6">
+      <c r="H7" s="12">
         <v>1820</v>
       </c>
     </row>
+    <row r="8" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>